<commit_message>
mise à jour pins kicad et HSIS_ApaliPi
</commit_message>
<xml_diff>
--- a/HSIS_ApaliPi.xlsx
+++ b/HSIS_ApaliPi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5950fb4c47a89ac9/Documents/Side_Projects/ApaliPi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="8_{FAFCA29F-FDD5-4983-9A6E-87E2D3D84178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B86126DB-9C19-43A7-8E9D-92A9B6F2859F}"/>
+  <xr:revisionPtr revIDLastSave="248" documentId="8_{FAFCA29F-FDD5-4983-9A6E-87E2D3D84178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F370BCCF-735E-4174-9A1B-9CAEBC595ED6}"/>
   <bookViews>
-    <workbookView xWindow="-2025" yWindow="120" windowWidth="16605" windowHeight="13755" xr2:uid="{FA17B988-1CAB-440E-A576-6CE1F6D73E4A}"/>
+    <workbookView xWindow="345" yWindow="465" windowWidth="16605" windowHeight="13755" xr2:uid="{FA17B988-1CAB-440E-A576-6CE1F6D73E4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="93">
   <si>
     <t>Ethernet</t>
   </si>
@@ -323,6 +323,30 @@
   </si>
   <si>
     <t>BKL1_PMW</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -527,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -558,6 +582,15 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -567,15 +600,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -890,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6A3321-C9C9-44A8-8F4A-03297E3FB28E}">
-  <dimension ref="C3:V69"/>
+  <dimension ref="B3:V69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,34 +926,34 @@
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="U3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="U4" s="12"/>
       <c r="V4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C5" s="27" t="s">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C5" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="29"/>
-      <c r="P5" s="27" t="s">
+      <c r="D5" s="25"/>
+      <c r="E5" s="26"/>
+      <c r="P5" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="29"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="26"/>
       <c r="U5" s="23"/>
       <c r="V5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
@@ -938,17 +963,22 @@
       <c r="E6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="P6" s="24" t="s">
+      <c r="P6" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="26"/>
-    </row>
-    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="Q6" s="28"/>
+      <c r="R6" s="29"/>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
       <c r="E7" s="8" t="s">
         <v>12</v>
       </c>
@@ -962,11 +992,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
       <c r="E8" s="9" t="s">
         <v>13</v>
       </c>
@@ -978,11 +1010,16 @@
         <v>211</v>
       </c>
     </row>
-    <row r="9" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
       <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1">
+        <v>3</v>
+      </c>
       <c r="E9" s="8" t="s">
         <v>14</v>
       </c>
@@ -994,25 +1031,32 @@
         <v>209</v>
       </c>
     </row>
-    <row r="10" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="30">
+        <v>6</v>
+      </c>
       <c r="E10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="P10" s="24" t="s">
+      <c r="P10" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="26"/>
-    </row>
-    <row r="11" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="Q10" s="28"/>
+      <c r="R10" s="29"/>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
       <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="30">
+        <v>4</v>
+      </c>
       <c r="E11" s="8" t="s">
         <v>16</v>
       </c>
@@ -1025,11 +1069,13 @@
         <v>207</v>
       </c>
     </row>
-    <row r="12" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="30">
+        <v>5</v>
+      </c>
       <c r="E12" s="9" t="s">
         <v>17</v>
       </c>
@@ -1041,25 +1087,32 @@
         <v>205</v>
       </c>
     </row>
-    <row r="13" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>92</v>
+      </c>
       <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="30">
+        <v>7</v>
+      </c>
       <c r="E13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="P13" s="24" t="s">
+      <c r="P13" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="26"/>
-    </row>
-    <row r="14" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q13" s="28"/>
+      <c r="R13" s="29"/>
+    </row>
+    <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="5"/>
+      <c r="D14" s="5">
+        <v>8</v>
+      </c>
       <c r="E14" s="10" t="s">
         <v>19</v>
       </c>
@@ -1071,7 +1124,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1083,15 +1136,15 @@
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="P16" s="24" t="s">
+      <c r="P16" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="26"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="29"/>
     </row>
     <row r="17" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
@@ -1118,11 +1171,11 @@
       </c>
     </row>
     <row r="19" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="29"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="26"/>
     </row>
     <row r="20" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
@@ -1139,7 +1192,9 @@
       <c r="C21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
       <c r="E21" s="3">
         <v>222</v>
       </c>
@@ -1148,35 +1203,41 @@
       <c r="C22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="1"/>
+      <c r="D22" s="1">
+        <v>3</v>
+      </c>
       <c r="E22" s="3">
         <v>224</v>
       </c>
-      <c r="P22" s="27" t="s">
+      <c r="P22" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="Q22" s="28"/>
-      <c r="R22" s="29"/>
+      <c r="Q22" s="25"/>
+      <c r="R22" s="26"/>
     </row>
     <row r="23" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C23" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="1"/>
+      <c r="D23" s="1">
+        <v>4</v>
+      </c>
       <c r="E23" s="3">
         <v>228</v>
       </c>
-      <c r="P23" s="24" t="s">
+      <c r="P23" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="Q23" s="25"/>
-      <c r="R23" s="26"/>
+      <c r="Q23" s="28"/>
+      <c r="R23" s="29"/>
     </row>
     <row r="24" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="1"/>
+      <c r="D24" s="30">
+        <v>6</v>
+      </c>
       <c r="E24" s="3">
         <v>230</v>
       </c>
@@ -1194,7 +1255,9 @@
       <c r="C25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="1"/>
+      <c r="D25" s="30">
+        <v>7</v>
+      </c>
       <c r="E25" s="3">
         <v>234</v>
       </c>
@@ -1210,7 +1273,9 @@
       <c r="C26" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="1"/>
+      <c r="D26" s="30">
+        <v>9</v>
+      </c>
       <c r="E26" s="3">
         <v>236</v>
       </c>
@@ -1229,7 +1294,9 @@
       <c r="C27" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="1"/>
+      <c r="D27" s="30">
+        <v>10</v>
+      </c>
       <c r="E27" s="3">
         <v>240</v>
       </c>
@@ -1245,7 +1312,9 @@
       <c r="C28" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="1"/>
+      <c r="D28" s="30">
+        <v>12</v>
+      </c>
       <c r="E28" s="3">
         <v>242</v>
       </c>
@@ -1261,21 +1330,25 @@
       <c r="C29" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="1"/>
+      <c r="D29" s="30">
+        <v>19</v>
+      </c>
       <c r="E29" s="14">
         <v>232</v>
       </c>
-      <c r="P29" s="24" t="s">
+      <c r="P29" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="Q29" s="25"/>
-      <c r="R29" s="26"/>
+      <c r="Q29" s="28"/>
+      <c r="R29" s="29"/>
     </row>
     <row r="30" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C30" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="1"/>
+      <c r="D30" s="30">
+        <v>13</v>
+      </c>
       <c r="E30" s="14">
         <v>220</v>
       </c>
@@ -1291,7 +1364,9 @@
       <c r="C31" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="11"/>
+      <c r="D31" s="11">
+        <v>15</v>
+      </c>
       <c r="E31" s="16">
         <v>207</v>
       </c>
@@ -1307,7 +1382,9 @@
       <c r="C32" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="18"/>
+      <c r="D32" s="18">
+        <v>16</v>
+      </c>
       <c r="E32" s="19">
         <v>205</v>
       </c>
@@ -1330,11 +1407,11 @@
     </row>
     <row r="35" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="27" t="s">
+      <c r="C36" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="D36" s="28"/>
-      <c r="E36" s="29"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="26"/>
     </row>
     <row r="37" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C37" s="2" t="s">
@@ -1346,11 +1423,11 @@
       <c r="E37" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="P37" s="27" t="s">
+      <c r="P37" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="Q37" s="28"/>
-      <c r="R37" s="29"/>
+      <c r="Q37" s="25"/>
+      <c r="R37" s="26"/>
     </row>
     <row r="38" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C38" s="2" t="s">
@@ -1360,11 +1437,11 @@
       <c r="E38" s="3">
         <v>163</v>
       </c>
-      <c r="P38" s="24" t="s">
+      <c r="P38" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="Q38" s="25"/>
-      <c r="R38" s="26"/>
+      <c r="Q38" s="28"/>
+      <c r="R38" s="29"/>
     </row>
     <row r="39" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C39" s="2" t="s">
@@ -1424,11 +1501,11 @@
       <c r="E42" s="3">
         <v>151</v>
       </c>
-      <c r="P42" s="24" t="s">
+      <c r="P42" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="Q42" s="25"/>
-      <c r="R42" s="26"/>
+      <c r="Q42" s="28"/>
+      <c r="R42" s="29"/>
     </row>
     <row r="43" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C43" s="2" t="s">
@@ -1490,11 +1567,11 @@
       </c>
     </row>
     <row r="48" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="P48" s="27" t="s">
+      <c r="P48" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="Q48" s="28"/>
-      <c r="R48" s="29"/>
+      <c r="Q48" s="25"/>
+      <c r="R48" s="26"/>
     </row>
     <row r="49" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P49" s="2" t="s">
@@ -1508,11 +1585,11 @@
       </c>
     </row>
     <row r="50" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C50" s="27" t="s">
+      <c r="C50" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="D50" s="28"/>
-      <c r="E50" s="29"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="26"/>
       <c r="P50" s="2" t="s">
         <v>74</v>
       </c>
@@ -1522,11 +1599,11 @@
       </c>
     </row>
     <row r="51" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C51" s="24" t="s">
+      <c r="C51" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="D51" s="25"/>
-      <c r="E51" s="26"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="29"/>
       <c r="P51" s="2" t="s">
         <v>75</v>
       </c>
@@ -1557,7 +1634,9 @@
       <c r="C53" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D53" s="1"/>
+      <c r="D53" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="E53" s="3">
         <v>80</v>
       </c>
@@ -1573,7 +1652,9 @@
       <c r="C54" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D54" s="1"/>
+      <c r="D54" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="E54" s="3">
         <v>82</v>
       </c>
@@ -1586,11 +1667,11 @@
       </c>
     </row>
     <row r="55" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C55" s="24" t="s">
+      <c r="C55" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="D55" s="25"/>
-      <c r="E55" s="26"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="29"/>
       <c r="P55" s="2" t="s">
         <v>79</v>
       </c>
@@ -1603,7 +1684,9 @@
       <c r="C56" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D56" s="1"/>
+      <c r="D56" s="30" t="s">
+        <v>87</v>
+      </c>
       <c r="E56" s="3">
         <v>86</v>
       </c>
@@ -1619,7 +1702,9 @@
       <c r="C57" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D57" s="5"/>
+      <c r="D57" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="E57" s="6">
         <v>88</v>
       </c>
@@ -1633,11 +1718,11 @@
     </row>
     <row r="59" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="60" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C60" s="27" t="s">
+      <c r="C60" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="D60" s="28"/>
-      <c r="E60" s="29"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="26"/>
     </row>
     <row r="61" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C61" s="2" t="s">
@@ -1724,11 +1809,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="P48:R48"/>
-    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="P42:R42"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="P23:R23"/>
+    <mergeCell ref="P29:R29"/>
+    <mergeCell ref="P37:R37"/>
+    <mergeCell ref="P38:R38"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="P5:R5"/>
@@ -1736,13 +1823,11 @@
     <mergeCell ref="P10:R10"/>
     <mergeCell ref="P13:R13"/>
     <mergeCell ref="P16:R16"/>
-    <mergeCell ref="P42:R42"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="P23:R23"/>
-    <mergeCell ref="P29:R29"/>
-    <mergeCell ref="P37:R37"/>
-    <mergeCell ref="P38:R38"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="P48:R48"/>
+    <mergeCell ref="C60:E60"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
PINOUT SD pas de modif KiCAD
</commit_message>
<xml_diff>
--- a/HSIS_ApaliPi.xlsx
+++ b/HSIS_ApaliPi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neile\OneDrive\Documents\Side_Projects\ApaliPi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D8F3F2-2810-43F1-98E7-A99DC5FC313F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A4D3F8-0EC5-4C84-8A10-A27E5E4541C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="810" windowWidth="16605" windowHeight="13755" xr2:uid="{FA17B988-1CAB-440E-A576-6CE1F6D73E4A}"/>
+    <workbookView xWindow="1035" yWindow="1155" windowWidth="16605" windowHeight="13755" xr2:uid="{FA17B988-1CAB-440E-A576-6CE1F6D73E4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="102">
   <si>
     <t>Ethernet</t>
   </si>
@@ -371,6 +371,9 @@
   </si>
   <si>
     <t>D3</t>
+  </si>
+  <si>
+    <t>card detection</t>
   </si>
 </sst>
 </file>
@@ -409,7 +412,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -449,6 +452,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -575,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -607,6 +616,15 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -616,15 +634,14 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -941,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6A3321-C9C9-44A8-8F4A-03297E3FB28E}">
   <dimension ref="B3:V79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L72" sqref="L72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,16 +979,16 @@
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="30"/>
-      <c r="P5" s="28" t="s">
+      <c r="D5" s="26"/>
+      <c r="E5" s="27"/>
+      <c r="P5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="30"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="27"/>
       <c r="U5" s="23"/>
       <c r="V5" t="s">
         <v>41</v>
@@ -987,11 +1004,11 @@
       <c r="E6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="P6" s="25" t="s">
+      <c r="P6" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="Q6" s="26"/>
-      <c r="R6" s="27"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="30"/>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -1065,11 +1082,11 @@
       <c r="E10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="P10" s="25" t="s">
+      <c r="P10" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="27"/>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="30"/>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -1124,11 +1141,11 @@
       <c r="E13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="P13" s="25" t="s">
+      <c r="P13" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="27"/>
+      <c r="Q13" s="29"/>
+      <c r="R13" s="30"/>
     </row>
     <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="4" t="s">
@@ -1164,11 +1181,11 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="P16" s="25" t="s">
+      <c r="P16" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="Q16" s="26"/>
-      <c r="R16" s="27"/>
+      <c r="Q16" s="29"/>
+      <c r="R16" s="30"/>
     </row>
     <row r="17" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
@@ -1195,11 +1212,11 @@
       </c>
     </row>
     <row r="19" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="29"/>
-      <c r="E19" s="30"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="27"/>
     </row>
     <row r="20" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
@@ -1233,11 +1250,11 @@
       <c r="E22" s="3">
         <v>224</v>
       </c>
-      <c r="P22" s="28" t="s">
+      <c r="P22" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="Q22" s="29"/>
-      <c r="R22" s="30"/>
+      <c r="Q22" s="26"/>
+      <c r="R22" s="27"/>
     </row>
     <row r="23" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C23" s="2" t="s">
@@ -1249,11 +1266,11 @@
       <c r="E23" s="3">
         <v>228</v>
       </c>
-      <c r="P23" s="25" t="s">
+      <c r="P23" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="Q23" s="26"/>
-      <c r="R23" s="27"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="30"/>
     </row>
     <row r="24" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
@@ -1360,11 +1377,11 @@
       <c r="E29" s="14">
         <v>232</v>
       </c>
-      <c r="P29" s="25" t="s">
+      <c r="P29" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="Q29" s="26"/>
-      <c r="R29" s="27"/>
+      <c r="Q29" s="29"/>
+      <c r="R29" s="30"/>
     </row>
     <row r="30" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C30" s="13" t="s">
@@ -1431,11 +1448,11 @@
     </row>
     <row r="35" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="28" t="s">
+      <c r="C36" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="D36" s="29"/>
-      <c r="E36" s="30"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="27"/>
     </row>
     <row r="37" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C37" s="2" t="s">
@@ -1447,11 +1464,11 @@
       <c r="E37" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="P37" s="28" t="s">
+      <c r="P37" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="Q37" s="29"/>
-      <c r="R37" s="30"/>
+      <c r="Q37" s="26"/>
+      <c r="R37" s="27"/>
     </row>
     <row r="38" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C38" s="2" t="s">
@@ -1461,11 +1478,11 @@
       <c r="E38" s="3">
         <v>163</v>
       </c>
-      <c r="P38" s="25" t="s">
+      <c r="P38" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="Q38" s="26"/>
-      <c r="R38" s="27"/>
+      <c r="Q38" s="29"/>
+      <c r="R38" s="30"/>
     </row>
     <row r="39" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C39" s="2" t="s">
@@ -1525,11 +1542,11 @@
       <c r="E42" s="3">
         <v>151</v>
       </c>
-      <c r="P42" s="25" t="s">
+      <c r="P42" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="Q42" s="26"/>
-      <c r="R42" s="27"/>
+      <c r="Q42" s="29"/>
+      <c r="R42" s="30"/>
     </row>
     <row r="43" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C43" s="2" t="s">
@@ -1591,11 +1608,11 @@
       </c>
     </row>
     <row r="48" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="P48" s="28" t="s">
+      <c r="P48" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="Q48" s="29"/>
-      <c r="R48" s="30"/>
+      <c r="Q48" s="26"/>
+      <c r="R48" s="27"/>
     </row>
     <row r="49" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P49" s="2" t="s">
@@ -1609,11 +1626,11 @@
       </c>
     </row>
     <row r="50" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C50" s="28" t="s">
+      <c r="C50" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D50" s="29"/>
-      <c r="E50" s="30"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="27"/>
       <c r="P50" s="2" t="s">
         <v>74</v>
       </c>
@@ -1623,11 +1640,11 @@
       </c>
     </row>
     <row r="51" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C51" s="25" t="s">
+      <c r="C51" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="D51" s="26"/>
-      <c r="E51" s="27"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="30"/>
       <c r="P51" s="2" t="s">
         <v>75</v>
       </c>
@@ -1691,11 +1708,11 @@
       </c>
     </row>
     <row r="55" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C55" s="25" t="s">
+      <c r="C55" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="D55" s="26"/>
-      <c r="E55" s="27"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="30"/>
       <c r="P55" s="2" t="s">
         <v>79</v>
       </c>
@@ -1742,11 +1759,11 @@
     </row>
     <row r="59" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="60" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C60" s="28" t="s">
+      <c r="C60" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="D60" s="29"/>
-      <c r="E60" s="30"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="27"/>
     </row>
     <row r="61" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C61" s="2" t="s">
@@ -1786,7 +1803,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C65" s="2" t="s">
         <v>56</v>
       </c>
@@ -1795,7 +1812,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C66" s="2" t="s">
         <v>58</v>
       </c>
@@ -1804,7 +1821,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C67" s="2" t="s">
         <v>59</v>
       </c>
@@ -1813,7 +1830,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="68" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C68" s="2" t="s">
         <v>60</v>
       </c>
@@ -1822,7 +1839,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="69" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C69" s="4" t="s">
         <v>61</v>
       </c>
@@ -1831,15 +1848,15 @@
         <v>113</v>
       </c>
     </row>
-    <row r="70" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="71" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C71" s="28" t="s">
+    <row r="70" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C71" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="D71" s="29"/>
-      <c r="E71" s="30"/>
-    </row>
-    <row r="72" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D71" s="26"/>
+      <c r="E71" s="27"/>
+    </row>
+    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C72" s="2" t="s">
         <v>5</v>
       </c>
@@ -1850,77 +1867,97 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C73" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D73" s="1"/>
+      <c r="D73" s="34">
+        <v>2</v>
+      </c>
       <c r="E73" s="3">
         <v>190</v>
       </c>
-    </row>
-    <row r="74" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F73" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="G73" s="31"/>
+    </row>
+    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C74" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D74" s="1"/>
+      <c r="D74" s="1">
+        <v>5</v>
+      </c>
       <c r="E74" s="3">
         <v>184</v>
       </c>
     </row>
-    <row r="75" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C75" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D75" s="1"/>
+      <c r="D75" s="1">
+        <v>3</v>
+      </c>
       <c r="E75" s="3">
         <v>180</v>
       </c>
     </row>
-    <row r="76" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C76" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D76" s="1"/>
+      <c r="D76" s="1">
+        <v>7</v>
+      </c>
       <c r="E76" s="3">
         <v>186</v>
       </c>
     </row>
-    <row r="77" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C77" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D77" s="1"/>
+      <c r="D77" s="24">
+        <v>8</v>
+      </c>
       <c r="E77" s="3">
         <v>188</v>
       </c>
     </row>
-    <row r="78" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C78" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D78" s="1"/>
+      <c r="D78" s="24">
+        <v>1</v>
+      </c>
       <c r="E78" s="3">
         <v>176</v>
       </c>
     </row>
-    <row r="79" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C79" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D79" s="5"/>
+      <c r="D79" s="33">
+        <v>2</v>
+      </c>
       <c r="E79" s="6">
         <v>178</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="P48:R48"/>
-    <mergeCell ref="C60:E60"/>
+  <mergeCells count="21">
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="P42:R42"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="P23:R23"/>
+    <mergeCell ref="P29:R29"/>
+    <mergeCell ref="P37:R37"/>
+    <mergeCell ref="P38:R38"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="P5:R5"/>
@@ -1928,13 +1965,12 @@
     <mergeCell ref="P10:R10"/>
     <mergeCell ref="P13:R13"/>
     <mergeCell ref="P16:R16"/>
-    <mergeCell ref="P42:R42"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="P23:R23"/>
-    <mergeCell ref="P29:R29"/>
-    <mergeCell ref="P37:R37"/>
-    <mergeCell ref="P38:R38"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="P48:R48"/>
+    <mergeCell ref="C60:E60"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>